<commit_message>
Stock data scraping to excel files
</commit_message>
<xml_diff>
--- a/files/Inputs.xlsx
+++ b/files/Inputs.xlsx
@@ -1,14 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24729"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24701"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6DEF4CD6-A2C8-466C-974B-E071F68AE334}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\moldo\Desktop\RPA\Project\TradingRobot\files\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99EE0B0A-6D7A-4093-AAAF-7C9A7173945F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="emails" sheetId="1" r:id="rId1"/>
+    <sheet name="website" sheetId="3" r:id="rId2"/>
+    <sheet name="symbols" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -26,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>Email</t>
   </si>
@@ -38,13 +45,46 @@
   </si>
   <si>
     <t>ioana.ilinca.moldovan@gmail.com</t>
+  </si>
+  <si>
+    <t>moldovanandrei2301@gmail.com</t>
+  </si>
+  <si>
+    <t>amoldovan65@yahoo.com</t>
+  </si>
+  <si>
+    <t>Symbols</t>
+  </si>
+  <si>
+    <t>NASDAQ-AMZN</t>
+  </si>
+  <si>
+    <t>NASDAQ-AAPL</t>
+  </si>
+  <si>
+    <t>NASDAQ-TSLA</t>
+  </si>
+  <si>
+    <t>NASDAQ-NFLX</t>
+  </si>
+  <si>
+    <t>BTCUSD</t>
+  </si>
+  <si>
+    <t>OTC-ETHE</t>
+  </si>
+  <si>
+    <t>Website Format</t>
+  </si>
+  <si>
+    <t>https://www.tradingview.com/symbols/{symbol}/technicals/</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -400,35 +440,45 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:A4"/>
+  <dimension ref="A1:A6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="32" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:1">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:1">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -436,7 +486,93 @@
     <hyperlink ref="A2" r:id="rId1" xr:uid="{8B84254C-5CAE-4AB0-9BA7-CAFBD1CF33BD}"/>
     <hyperlink ref="A3" r:id="rId2" xr:uid="{639FA377-53E6-4EC6-B9DD-4F836FE24028}"/>
     <hyperlink ref="A4" r:id="rId3" xr:uid="{0DFF48A4-574B-495C-BBCA-2FFFDA7C03ED}"/>
+    <hyperlink ref="A5" r:id="rId4" xr:uid="{583DC358-047F-4DFA-8E63-D39D19FE8395}"/>
+    <hyperlink ref="A6" r:id="rId5" xr:uid="{53752678-02F8-47BA-A927-27E396FCBB68}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4C38828-54A8-41DA-9513-917644668FBE}">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="56.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{41F7FEC7-2DA5-4DDD-A970-F0BEFC73CAD1}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{20D6C9CC-91A2-4CBA-AB72-87215434A8F0}">
+  <dimension ref="A1:A7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="17.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>